<commit_message>
fixed no indices error
</commit_message>
<xml_diff>
--- a/results/21_3_8 Experiment - Instance Based Sweeping/c0_s1_1_per_client_fgsm.xlsx
+++ b/results/21_3_8 Experiment - Instance Based Sweeping/c0_s1_1_per_client_fgsm.xlsx
@@ -435,16 +435,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8890000581741333</v>
+        <v>0.9020000696182251</v>
       </c>
       <c r="C2">
-        <v>0.7940000295639038</v>
+        <v>0.8020000457763672</v>
       </c>
       <c r="D2">
-        <v>0.7780000567436218</v>
+        <v>0.7950000166893005</v>
       </c>
       <c r="E2">
-        <v>0.8550000190734863</v>
+        <v>0.8530000448226929</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -455,13 +455,13 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>0.8450000286102295</v>
+      </c>
+      <c r="D3">
         <v>0.8330000638961792</v>
       </c>
-      <c r="D3">
-        <v>0.8280000686645508</v>
-      </c>
       <c r="E3">
-        <v>0.8880000710487366</v>
+        <v>0.8860000371932983</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -469,16 +469,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.9220607876777649</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.798155665397644</v>
+        <v>0.7994269728660583</v>
       </c>
       <c r="D4">
-        <v>0.792610228061676</v>
+        <v>0.7939913868904114</v>
       </c>
       <c r="E4">
-        <v>0.8715696930885315</v>
+        <v>0.8428571224212646</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -489,13 +489,13 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.8319671750068665</v>
+        <v>0.830945611000061</v>
       </c>
       <c r="D5">
-        <v>0.8414779305458069</v>
+        <v>0.8283261656761169</v>
       </c>
       <c r="E5">
-        <v>0.9034028649330139</v>
+        <v>0.8285714387893677</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -503,16 +503,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.7860081791877747</v>
+        <v>0.9018036127090454</v>
       </c>
       <c r="C6">
-        <v>0.625</v>
+        <v>0.8033794164657593</v>
       </c>
       <c r="D6">
-        <v>0.7018633484840393</v>
+        <v>0.795306384563446</v>
       </c>
       <c r="E6">
-        <v>0.6853932738304138</v>
+        <v>0.8537634611129761</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -520,16 +520,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.9999999403953552</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0.875</v>
+        <v>0.8525345325469971</v>
       </c>
       <c r="D7">
-        <v>0.7577639818191528</v>
+        <v>0.8344197869300842</v>
       </c>
       <c r="E7">
-        <v>0.7303370833396912</v>
+        <v>0.8903226256370544</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -540,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.1960000097751617</v>
+        <v>0.6500000357627869</v>
       </c>
       <c r="D8">
-        <v>0.2550000250339508</v>
+        <v>0.7660000324249268</v>
       </c>
       <c r="E8">
-        <v>0.2700000107288361</v>
+        <v>0.9290000200271606</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -554,16 +554,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.2430000156164169</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="C9">
-        <v>0.02400000020861626</v>
+        <v>0.6510000228881836</v>
       </c>
       <c r="D9">
-        <v>0.1610000133514404</v>
+        <v>0.7670000195503235</v>
       </c>
       <c r="E9">
-        <v>0.08900000154972076</v>
+        <v>0.9300000667572021</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -574,13 +574,13 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1.085583686828613</v>
+        <v>1.069687604904175</v>
       </c>
       <c r="D10">
-        <v>1.093605041503906</v>
+        <v>1.119789004325867</v>
       </c>
       <c r="E10">
-        <v>0.9750272631645203</v>
+        <v>0.9930899143218994</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -588,16 +588,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.0006905339541845024</v>
       </c>
       <c r="C11">
-        <v>1.080765724182129</v>
+        <v>1.085886120796204</v>
       </c>
       <c r="D11">
-        <v>1.148160934448242</v>
+        <v>1.204179525375366</v>
       </c>
       <c r="E11">
-        <v>0.9944726228713989</v>
+        <v>1.061654448509216</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -608,13 +608,13 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1.085583686828613</v>
+        <v>1.069687604904175</v>
       </c>
       <c r="D12">
-        <v>1.093605041503906</v>
+        <v>1.119789004325867</v>
       </c>
       <c r="E12">
-        <v>0.9750272631645203</v>
+        <v>0.9930899143218994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>